<commit_message>
Adding doc resources and visualisation examples with ggplot
</commit_message>
<xml_diff>
--- a/workshop/R code/01 session/SimData.xlsx
+++ b/workshop/R code/01 session/SimData.xlsx
@@ -45,7 +45,7 @@
     <numFmt numFmtId="166" formatCode="0.00_);\(0.00\)"/>
     <numFmt numFmtId="167" formatCode="0.000_);\(0.000\)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -56,6 +56,30 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -78,11 +102,39 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -91,13 +143,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -105,9 +157,49 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="30">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -437,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E290"/>
+  <dimension ref="A1:J290"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -450,26 +542,30 @@
     <col min="3" max="3" width="21.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="21.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="20.83203125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" style="11" customWidth="1"/>
+    <col min="10" max="10" width="15" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="5" customFormat="1">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:10" s="3" customFormat="1">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="I1" s="10"/>
+      <c r="J1" s="4"/>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="7">
         <v>2014</v>
       </c>
@@ -486,7 +582,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:10">
       <c r="A3" s="7">
         <v>2014.125</v>
       </c>
@@ -503,7 +599,7 @@
         <v>505625</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:10">
       <c r="A4" s="7">
         <v>2014.25</v>
       </c>
@@ -520,7 +616,7 @@
         <v>511230</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:10">
       <c r="A5" s="7">
         <v>2014.375</v>
       </c>
@@ -537,7 +633,7 @@
         <v>516816</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:10">
       <c r="A6" s="7">
         <v>2014.5</v>
       </c>
@@ -554,7 +650,7 @@
         <v>522383</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:10">
       <c r="A7" s="7">
         <v>2014.625</v>
       </c>
@@ -571,7 +667,7 @@
         <v>527930</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:10">
       <c r="A8" s="7">
         <v>2014.75</v>
       </c>
@@ -587,8 +683,10 @@
       <c r="E8" s="6">
         <v>533457</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="I8"/>
+      <c r="J8"/>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="7">
         <v>2014.875</v>
       </c>
@@ -604,8 +702,10 @@
       <c r="E9" s="6">
         <v>538966</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="I9"/>
+      <c r="J9"/>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="7">
         <v>2015</v>
       </c>
@@ -621,8 +721,10 @@
       <c r="E10" s="6">
         <v>544455</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="I10"/>
+      <c r="J10"/>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="7">
         <v>2015.125</v>
       </c>
@@ -638,8 +740,10 @@
       <c r="E11" s="6">
         <v>549925</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="I11"/>
+      <c r="J11"/>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="7">
         <v>2015.25</v>
       </c>
@@ -655,8 +759,10 @@
       <c r="E12" s="6">
         <v>555376</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="I12"/>
+      <c r="J12"/>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="7">
         <v>2015.375</v>
       </c>
@@ -673,7 +779,7 @@
         <v>560808</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:10">
       <c r="A14" s="7">
         <v>2015.5</v>
       </c>
@@ -690,7 +796,7 @@
         <v>566222</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:10">
       <c r="A15" s="7">
         <v>2015.625</v>
       </c>
@@ -707,7 +813,7 @@
         <v>571616</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:10">
       <c r="A16" s="7">
         <v>2015.75</v>
       </c>
@@ -5384,6 +5490,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>